<commit_message>
Rerun NPCC contingency analysis cases
</commit_message>
<xml_diff>
--- a/src/notes/lmp/data/npcc_base.xlsx
+++ b/src/notes/lmp/data/npcc_base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/psal/src/notes/lmp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C727F746-D993-FD48-A675-77A0B0AE80B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C426D831-44F0-5442-9EBD-ECC91F2FC05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="7420" windowWidth="21600" windowHeight="18940" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="7420" windowWidth="21600" windowHeight="18940" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -16304,9 +16304,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="165" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="3" sqref="A3:XFD3 A5:XFD5 A6:XFD6 A9:XFD25"/>
+    <sheetView zoomScale="165" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M9" activeCellId="3" sqref="M3:N3 M5:N5 M6:N6 M9:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16724,7 +16724,7 @@
         <v>0.03</v>
       </c>
       <c r="M7">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -17873,8 +17873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22EDBF59-3AD7-7F42-811C-1C55C6835A6B}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18015,7 +18015,7 @@
         <v>839</v>
       </c>
       <c r="U2" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V2" t="s">
         <v>840</v>
@@ -18089,7 +18089,7 @@
         <v>839</v>
       </c>
       <c r="U3" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V3" t="s">
         <v>840</v>
@@ -18163,7 +18163,7 @@
         <v>839</v>
       </c>
       <c r="U4" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V4" t="s">
         <v>840</v>
@@ -18237,7 +18237,7 @@
         <v>839</v>
       </c>
       <c r="U5" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V5" t="s">
         <v>840</v>
@@ -18311,7 +18311,7 @@
         <v>839</v>
       </c>
       <c r="U6" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V6" t="s">
         <v>840</v>
@@ -18386,7 +18386,7 @@
         <v>4.2</v>
       </c>
       <c r="U7" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V7" s="4">
         <v>0.1</v>
@@ -18461,7 +18461,7 @@
         <v>4.2</v>
       </c>
       <c r="U8" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V8" s="4">
         <v>0.1</v>
@@ -18535,7 +18535,7 @@
         <v>839</v>
       </c>
       <c r="U9" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V9" t="s">
         <v>840</v>
@@ -18609,7 +18609,7 @@
         <v>839</v>
       </c>
       <c r="U10" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V10" t="s">
         <v>840</v>
@@ -18683,7 +18683,7 @@
         <v>839</v>
       </c>
       <c r="U11" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V11" t="s">
         <v>840</v>
@@ -18757,7 +18757,7 @@
         <v>839</v>
       </c>
       <c r="U12" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V12" t="s">
         <v>840</v>
@@ -18831,7 +18831,7 @@
         <v>839</v>
       </c>
       <c r="U13" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V13" t="s">
         <v>840</v>
@@ -18905,7 +18905,7 @@
         <v>839</v>
       </c>
       <c r="U14" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V14" t="s">
         <v>840</v>
@@ -18979,7 +18979,7 @@
         <v>4.2</v>
       </c>
       <c r="U15" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V15" s="4">
         <v>0.1</v>
@@ -19053,7 +19053,7 @@
         <v>4.2</v>
       </c>
       <c r="U16" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V16" s="4">
         <v>0.1</v>
@@ -19127,7 +19127,7 @@
         <v>891</v>
       </c>
       <c r="U17" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V17" t="s">
         <v>892</v>
@@ -19201,7 +19201,7 @@
         <v>839</v>
       </c>
       <c r="U18" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V18" t="s">
         <v>840</v>
@@ -19275,7 +19275,7 @@
         <v>839</v>
       </c>
       <c r="U19" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V19" t="s">
         <v>840</v>
@@ -19349,7 +19349,7 @@
         <v>839</v>
       </c>
       <c r="U20" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V20" t="s">
         <v>840</v>
@@ -19423,7 +19423,7 @@
         <v>839</v>
       </c>
       <c r="U21" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V21" t="s">
         <v>840</v>
@@ -19497,7 +19497,7 @@
         <v>839</v>
       </c>
       <c r="U22" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V22" t="s">
         <v>840</v>
@@ -19571,7 +19571,7 @@
         <v>4.2</v>
       </c>
       <c r="U23" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V23" s="4">
         <v>0.1</v>
@@ -19645,7 +19645,7 @@
         <v>4.2</v>
       </c>
       <c r="U24" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V24" s="4">
         <v>0.1</v>
@@ -19719,7 +19719,7 @@
         <v>895</v>
       </c>
       <c r="U25" s="4">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="V25" t="s">
         <v>896</v>
@@ -23428,7 +23428,7 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26198,7 +26198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E62DA64-E676-1846-A857-DF8023B83120}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+    <sheetView zoomScale="134" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>